<commit_message>
feat: 1.5T data, analysis code and results
- batch analysis function and plotting
- 1.5T nifti data, segmentations and information spreadsheet
- results for method regionwise_bootstrap, 10,000 iterations
</commit_message>
<xml_diff>
--- a/data/1.5T/image_information.xlsx
+++ b/data/1.5T/image_information.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Users\Aaron\Seafile\GSPCD_Science\8025-NMR Thermometry\ethylene-glycol-phantom-thermometry\data\1.5T\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25927A70-FAE5-43E5-AAC2-540866B464F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8802B652-5699-4622-AAD2-E0ED23111FAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="10605" yWindow="0" windowWidth="18195" windowHeight="15600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="25">
   <si>
     <t>Meas_01_final</t>
   </si>
@@ -91,6 +91,15 @@
   </si>
   <si>
     <t>acquisition_duration</t>
+  </si>
+  <si>
+    <t>valid_segmentation</t>
+  </si>
+  <si>
+    <t>segmentation_01</t>
+  </si>
+  <si>
+    <t>segmentation_02</t>
   </si>
 </sst>
 </file>
@@ -417,10 +426,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F19"/>
+  <dimension ref="A1:G19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="G18" sqref="G18:G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -429,9 +438,11 @@
     <col min="2" max="2" width="54.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="64.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
@@ -450,8 +461,11 @@
       <c r="F1" s="1" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G1" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -470,8 +484,11 @@
       <c r="F2">
         <v>151</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -490,8 +507,11 @@
       <c r="F3">
         <v>151</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>0</v>
       </c>
@@ -510,8 +530,11 @@
       <c r="F4">
         <v>151</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>0</v>
       </c>
@@ -530,8 +553,11 @@
       <c r="F5">
         <v>151</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -550,8 +576,11 @@
       <c r="F6">
         <v>151</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -570,8 +599,11 @@
       <c r="F7">
         <v>151</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G7" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>9</v>
       </c>
@@ -590,8 +622,11 @@
       <c r="F8">
         <v>151</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -610,8 +645,11 @@
       <c r="F9">
         <v>151</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G9" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>11</v>
       </c>
@@ -630,8 +668,11 @@
       <c r="F10">
         <v>151</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G10" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>11</v>
       </c>
@@ -650,8 +691,11 @@
       <c r="F11">
         <v>151</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G11" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>13</v>
       </c>
@@ -670,8 +714,11 @@
       <c r="F12">
         <v>151</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G12" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>13</v>
       </c>
@@ -690,8 +737,11 @@
       <c r="F13">
         <v>151</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G13" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>15</v>
       </c>
@@ -710,8 +760,11 @@
       <c r="F14">
         <v>151</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G14" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>15</v>
       </c>
@@ -730,8 +783,11 @@
       <c r="F15">
         <v>151</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G15" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>15</v>
       </c>
@@ -750,8 +806,11 @@
       <c r="F16">
         <v>151</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G16" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>15</v>
       </c>
@@ -770,8 +829,11 @@
       <c r="F17">
         <v>151</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G17" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>17</v>
       </c>
@@ -790,8 +852,11 @@
       <c r="F18">
         <v>151</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G18" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>17</v>
       </c>
@@ -809,6 +874,9 @@
       </c>
       <c r="F19">
         <v>151</v>
+      </c>
+      <c r="G19" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>